<commit_message>
Latest Update April 2024
</commit_message>
<xml_diff>
--- a/CS-100/CS-104/Research/Temp.xlsx
+++ b/CS-100/CS-104/Research/Temp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myacg-my.sharepoint.com/personal/270168960_yoobeestudent_ac_nz/Documents/Assignments/CS-104/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myacg-my.sharepoint.com/personal/270168960_yoobeestudent_ac_nz/Documents/Assignments/CS-104/Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{A5B57014-AC7B-4779-A496-3845CA45A52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61B3C157-1F99-4436-AABE-F16B7DD2EB7D}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{A5B57014-AC7B-4779-A496-3845CA45A52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{800471B7-9FF5-489B-A928-50767D35812C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{626F58FB-CACA-4A59-A37A-12BE0F5BD874}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Time Taken</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 6</t>
   </si>
   <si>
     <t>Task 7</t>
@@ -82,18 +79,6 @@
     <t>Task Dificulty</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Tester</t>
   </si>
   <si>
@@ -110,6 +95,9 @@
   </si>
   <si>
     <t>Tester 5</t>
+  </si>
+  <si>
+    <t>Task 5</t>
   </si>
 </sst>
 </file>
@@ -367,7 +355,7 @@
                   <c:v>Task 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Task 6</c:v>
+                  <c:v>Task 5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Task 7</c:v>
@@ -388,28 +376,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>27.8</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.8</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.8</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.2</c:v>
+                  <c:v>18.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.1999999999999993</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -490,7 +478,7 @@
                   <c:v>Task 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Task 6</c:v>
+                  <c:v>Task 5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Task 7</c:v>
@@ -511,22 +499,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.8</c:v>
@@ -593,6 +581,8 @@
         <c:axId val="724397519"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.5"/>
+          <c:min val="0.8"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -721,7 +711,7 @@
                   <c:v>Task 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Task 6</c:v>
+                  <c:v>Task 5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Task 7</c:v>
@@ -742,22 +732,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.8</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.8</c:v>
@@ -912,7 +902,7 @@
                   <c:v>Task 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Task 6</c:v>
+                  <c:v>Task 5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Task 7</c:v>
@@ -933,28 +923,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>27.8</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.8</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>6.2</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.8</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.2</c:v>
+                  <c:v>18.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.1999999999999993</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1187,19 +1177,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1295,19 +1285,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>1.375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4</c:v>
+                  <c:v>1.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5</c:v>
+                  <c:v>1.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1387,7 +1377,8 @@
         <c:axId val="241812544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="5"/>
+          <c:max val="7"/>
+          <c:min val="3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1444,7 +1435,8 @@
         <c:axId val="1482022896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.8"/>
+          <c:max val="2"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1495,6 +1487,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1482022896"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2166,16 +2159,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>359338</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>121689</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>484149</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>55999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>59315</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>157432</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>184125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>78604</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2277,6 +2270,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2602,8 +2599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C918ECCE-38C8-45B7-8A89-8901D87EE963}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,10 +2615,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2629,10 +2626,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>27.8</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>2.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2640,10 +2637,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>11.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C3">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2651,10 +2648,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>12.2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2662,40 +2659,40 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>6.2</v>
+        <v>5.6</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4">
-        <v>15.8</v>
+        <v>6.2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>21.2</v>
+        <v>18.8</v>
       </c>
       <c r="C7">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>12.4</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>1.8</v>
@@ -2703,10 +2700,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>8.1999999999999993</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2715,68 +2712,68 @@
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>1.5</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>1.4</v>
+        <v>1.625</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>1.5</v>
+        <v>1.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>